<commit_message>
Add a datatable lookup(not working yet)
</commit_message>
<xml_diff>
--- a/Data for bank recon.xlsx
+++ b/Data for bank recon.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="BANK" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2469" uniqueCount="1378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="1375">
   <si>
     <t>Transaction Date</t>
   </si>
@@ -4157,15 +4157,6 @@
   </si>
   <si>
     <t>TYPE</t>
-  </si>
-  <si>
-    <t>NUMBER EMPTY</t>
-  </si>
-  <si>
-    <t>IS NUMERIC</t>
-  </si>
-  <si>
-    <t>NOT NUMERIC</t>
   </si>
 </sst>
 </file>
@@ -4638,9 +4629,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F291"/>
+  <dimension ref="A1:E291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="F13" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
@@ -4655,7 +4646,7 @@
     <col min="7" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>1370</v>
       </c>
@@ -4672,7 +4663,7 @@
         <v>1372</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>43818</v>
       </c>
@@ -4688,11 +4679,8 @@
       <c r="E2" s="15">
         <v>-3500000</v>
       </c>
-      <c r="F2" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13">
         <v>43818</v>
       </c>
@@ -4708,11 +4696,8 @@
       <c r="E3" s="15">
         <v>-3500000</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>43817</v>
       </c>
@@ -4728,11 +4713,8 @@
       <c r="E4" s="15">
         <v>-860</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>43815</v>
       </c>
@@ -4748,11 +4730,8 @@
       <c r="E5" s="15">
         <v>250</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>43812</v>
       </c>
@@ -4768,11 +4747,8 @@
       <c r="E6" s="15">
         <v>860</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>43812</v>
       </c>
@@ -4788,11 +4764,8 @@
       <c r="E7" s="15">
         <v>860</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>43812</v>
       </c>
@@ -4808,11 +4781,8 @@
       <c r="E8" s="15">
         <v>860</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>43812</v>
       </c>
@@ -4828,11 +4798,8 @@
       <c r="E9" s="15">
         <v>860</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="13">
         <v>43812</v>
       </c>
@@ -4848,11 +4815,8 @@
       <c r="E10" s="15">
         <v>860</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13">
         <v>43812</v>
       </c>
@@ -4868,11 +4832,8 @@
       <c r="E11" s="15">
         <v>860</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13">
         <v>43812</v>
       </c>
@@ -4888,11 +4849,8 @@
       <c r="E12" s="15">
         <v>860</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13">
         <v>43812</v>
       </c>
@@ -4908,11 +4866,8 @@
       <c r="E13" s="15">
         <v>860</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13">
         <v>43812</v>
       </c>
@@ -4928,11 +4883,8 @@
       <c r="E14" s="15">
         <v>860</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13">
         <v>43812</v>
       </c>
@@ -4948,11 +4900,8 @@
       <c r="E15" s="15">
         <v>860</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13">
         <v>43812</v>
       </c>
@@ -4968,11 +4917,8 @@
       <c r="E16" s="15">
         <v>860</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13">
         <v>43812</v>
       </c>
@@ -4988,11 +4934,8 @@
       <c r="E17" s="15">
         <v>860</v>
       </c>
-      <c r="F17" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13">
         <v>43812</v>
       </c>
@@ -5008,11 +4951,8 @@
       <c r="E18" s="15">
         <v>860</v>
       </c>
-      <c r="F18" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13">
         <v>43812</v>
       </c>
@@ -5028,11 +4968,8 @@
       <c r="E19" s="15">
         <v>860</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13">
         <v>43812</v>
       </c>
@@ -5048,11 +4985,8 @@
       <c r="E20" s="15">
         <v>860</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13">
         <v>43816</v>
       </c>
@@ -5068,11 +5002,8 @@
       <c r="E21" s="15">
         <v>860</v>
       </c>
-      <c r="F21" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="13">
         <v>43816</v>
       </c>
@@ -5088,11 +5019,8 @@
       <c r="E22" s="15">
         <v>860</v>
       </c>
-      <c r="F22" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13">
         <v>43816</v>
       </c>
@@ -5108,11 +5036,8 @@
       <c r="E23" s="15">
         <v>860</v>
       </c>
-      <c r="F23" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13">
         <v>43816</v>
       </c>
@@ -5128,11 +5053,8 @@
       <c r="E24" s="15">
         <v>860</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13">
         <v>43817</v>
       </c>
@@ -5148,11 +5070,8 @@
       <c r="E25" s="15">
         <v>860</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13">
         <v>43817</v>
       </c>
@@ -5168,11 +5087,8 @@
       <c r="E26" s="15">
         <v>860</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="13">
         <v>43817</v>
       </c>
@@ -5188,11 +5104,8 @@
       <c r="E27" s="15">
         <v>860</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13">
         <v>43817</v>
       </c>
@@ -5208,11 +5121,8 @@
       <c r="E28" s="15">
         <v>860</v>
       </c>
-      <c r="F28" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13">
         <v>43817</v>
       </c>
@@ -5228,11 +5138,8 @@
       <c r="E29" s="15">
         <v>860</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13">
         <v>43817</v>
       </c>
@@ -5248,11 +5155,8 @@
       <c r="E30" s="15">
         <v>860</v>
       </c>
-      <c r="F30" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="13">
         <v>43817</v>
       </c>
@@ -5268,11 +5172,8 @@
       <c r="E31" s="15">
         <v>860</v>
       </c>
-      <c r="F31" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13">
         <v>43817</v>
       </c>
@@ -5288,11 +5189,8 @@
       <c r="E32" s="15">
         <v>860</v>
       </c>
-      <c r="F32" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13">
         <v>43817</v>
       </c>
@@ -5308,11 +5206,8 @@
       <c r="E33" s="15">
         <v>860</v>
       </c>
-      <c r="F33" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13">
         <v>43817</v>
       </c>
@@ -5328,11 +5223,8 @@
       <c r="E34" s="15">
         <v>860</v>
       </c>
-      <c r="F34" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13">
         <v>43817</v>
       </c>
@@ -5348,11 +5240,8 @@
       <c r="E35" s="15">
         <v>860</v>
       </c>
-      <c r="F35" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13">
         <v>43817</v>
       </c>
@@ -5368,11 +5257,8 @@
       <c r="E36" s="15">
         <v>860</v>
       </c>
-      <c r="F36" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="13">
         <v>43817</v>
       </c>
@@ -5388,11 +5274,8 @@
       <c r="E37" s="15">
         <v>860</v>
       </c>
-      <c r="F37" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13">
         <v>43819</v>
       </c>
@@ -5408,11 +5291,8 @@
       <c r="E38" s="15">
         <v>860</v>
       </c>
-      <c r="F38" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="13">
         <v>43819</v>
       </c>
@@ -5428,11 +5308,8 @@
       <c r="E39" s="15">
         <v>860</v>
       </c>
-      <c r="F39" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="13">
         <v>43820</v>
       </c>
@@ -5448,11 +5325,8 @@
       <c r="E40" s="15">
         <v>860</v>
       </c>
-      <c r="F40" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="13">
         <v>43812</v>
       </c>
@@ -5468,11 +5342,8 @@
       <c r="E41" s="15">
         <v>1200</v>
       </c>
-      <c r="F41" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="13">
         <v>43816</v>
       </c>
@@ -5488,11 +5359,8 @@
       <c r="E42" s="15">
         <v>1200</v>
       </c>
-      <c r="F42" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="13">
         <v>43818</v>
       </c>
@@ -5508,11 +5376,8 @@
       <c r="E43" s="15">
         <v>2020</v>
       </c>
-      <c r="F43" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="13">
         <v>43818</v>
       </c>
@@ -5528,11 +5393,8 @@
       <c r="E44" s="15">
         <v>2705</v>
       </c>
-      <c r="F44" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" s="29" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:5" s="29" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="25">
         <v>43810</v>
       </c>
@@ -5548,11 +5410,8 @@
       <c r="E45" s="28">
         <v>3000</v>
       </c>
-      <c r="F45" s="29" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="13">
         <v>43812</v>
       </c>
@@ -5568,11 +5427,8 @@
       <c r="E46" s="15">
         <v>3556</v>
       </c>
-      <c r="F46" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="13">
         <v>43812</v>
       </c>
@@ -5588,11 +5444,8 @@
       <c r="E47" s="15">
         <v>3556</v>
       </c>
-      <c r="F47" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="13">
         <v>43812</v>
       </c>
@@ -5608,11 +5461,8 @@
       <c r="E48" s="15">
         <v>3556</v>
       </c>
-      <c r="F48" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="13">
         <v>43809</v>
       </c>
@@ -5628,11 +5478,8 @@
       <c r="E49" s="15">
         <v>3740</v>
       </c>
-      <c r="F49" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="13">
         <v>43817</v>
       </c>
@@ -5648,11 +5495,8 @@
       <c r="E50" s="15">
         <v>3800</v>
       </c>
-      <c r="F50" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="13">
         <v>43808</v>
       </c>
@@ -5668,11 +5512,8 @@
       <c r="E51" s="15">
         <v>3833</v>
       </c>
-      <c r="F51" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="13">
         <v>43808</v>
       </c>
@@ -5688,11 +5529,8 @@
       <c r="E52" s="15">
         <v>3890.65</v>
       </c>
-      <c r="F52" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="13">
         <v>43822</v>
       </c>
@@ -5708,11 +5546,8 @@
       <c r="E53" s="15">
         <v>3890.65</v>
       </c>
-      <c r="F53" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="13">
         <v>43805</v>
       </c>
@@ -5728,11 +5563,8 @@
       <c r="E54" s="15">
         <v>4001</v>
       </c>
-      <c r="F54" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="13">
         <v>43805</v>
       </c>
@@ -5748,11 +5580,8 @@
       <c r="E55" s="15">
         <v>4022</v>
       </c>
-      <c r="F55" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="13">
         <v>43812</v>
       </c>
@@ -5768,11 +5597,8 @@
       <c r="E56" s="15">
         <v>4200</v>
       </c>
-      <c r="F56" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="13">
         <v>43812</v>
       </c>
@@ -5788,11 +5614,8 @@
       <c r="E57" s="15">
         <v>5000</v>
       </c>
-      <c r="F57" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="13">
         <v>43819</v>
       </c>
@@ -5808,11 +5631,8 @@
       <c r="E58" s="15">
         <v>5210</v>
       </c>
-      <c r="F58" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="13">
         <v>43817</v>
       </c>
@@ -5828,11 +5648,8 @@
       <c r="E59" s="15">
         <v>5654</v>
       </c>
-      <c r="F59" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="13">
         <v>43816</v>
       </c>
@@ -5848,11 +5665,8 @@
       <c r="E60" s="15">
         <v>5748.2</v>
       </c>
-      <c r="F60" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="13">
         <v>43822</v>
       </c>
@@ -5868,11 +5682,8 @@
       <c r="E61" s="15">
         <v>5748.2</v>
       </c>
-      <c r="F61" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="13">
         <v>43817</v>
       </c>
@@ -5888,11 +5699,8 @@
       <c r="E62" s="15">
         <v>6010</v>
       </c>
-      <c r="F62" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="13">
         <v>43817</v>
       </c>
@@ -5908,11 +5716,8 @@
       <c r="E63" s="15">
         <v>6411</v>
       </c>
-      <c r="F63" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="13">
         <v>43812</v>
       </c>
@@ -5928,11 +5733,8 @@
       <c r="E64" s="15">
         <v>6880</v>
       </c>
-      <c r="F64" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="13">
         <v>43818</v>
       </c>
@@ -5948,11 +5750,8 @@
       <c r="E65" s="15">
         <v>6880</v>
       </c>
-      <c r="F65" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="13">
         <v>43818</v>
       </c>
@@ -5968,11 +5767,8 @@
       <c r="E66" s="15">
         <v>7079</v>
       </c>
-      <c r="F66" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="13">
         <v>43808</v>
       </c>
@@ -5988,11 +5784,8 @@
       <c r="E67" s="15">
         <v>8064</v>
       </c>
-      <c r="F67" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="13">
         <v>43817</v>
       </c>
@@ -6008,11 +5801,8 @@
       <c r="E68" s="15">
         <v>8905</v>
       </c>
-      <c r="F68" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="13">
         <v>43815</v>
       </c>
@@ -6028,11 +5818,8 @@
       <c r="E69" s="15">
         <v>9000</v>
       </c>
-      <c r="F69" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="13">
         <v>43820</v>
       </c>
@@ -6048,11 +5835,8 @@
       <c r="E70" s="15">
         <v>9660</v>
       </c>
-      <c r="F70" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="13">
         <v>43809</v>
       </c>
@@ -6068,11 +5852,8 @@
       <c r="E71" s="15">
         <v>9739</v>
       </c>
-      <c r="F71" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="13">
         <v>43822</v>
       </c>
@@ -6088,11 +5869,8 @@
       <c r="E72" s="15">
         <v>10000</v>
       </c>
-      <c r="F72" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="13">
         <v>43822</v>
       </c>
@@ -6108,11 +5886,8 @@
       <c r="E73" s="15">
         <v>10000</v>
       </c>
-      <c r="F73" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="13">
         <v>43822</v>
       </c>
@@ -6128,11 +5903,8 @@
       <c r="E74" s="15">
         <v>10000</v>
       </c>
-      <c r="F74" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="13">
         <v>43804</v>
       </c>
@@ -6148,11 +5920,8 @@
       <c r="E75" s="15">
         <v>10120</v>
       </c>
-      <c r="F75" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="13">
         <v>43812</v>
       </c>
@@ -6168,11 +5937,8 @@
       <c r="E76" s="15">
         <v>12600</v>
       </c>
-      <c r="F76" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="13">
         <v>43818</v>
       </c>
@@ -6188,11 +5954,8 @@
       <c r="E77" s="15">
         <v>13976.7</v>
       </c>
-      <c r="F77" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="13">
         <v>43804</v>
       </c>
@@ -6208,11 +5971,8 @@
       <c r="E78" s="15">
         <v>14780</v>
       </c>
-      <c r="F78" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="13">
         <v>43801</v>
       </c>
@@ -6228,11 +5988,8 @@
       <c r="E79" s="15">
         <v>15000</v>
       </c>
-      <c r="F79" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="13">
         <v>43819</v>
       </c>
@@ -6248,11 +6005,8 @@
       <c r="E80" s="15">
         <v>16340</v>
       </c>
-      <c r="F80" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="13">
         <v>43817</v>
       </c>
@@ -6268,11 +6022,8 @@
       <c r="E81" s="15">
         <v>17094</v>
       </c>
-      <c r="F81" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="13">
         <v>43822</v>
       </c>
@@ -6288,11 +6039,8 @@
       <c r="E82" s="15">
         <v>17371</v>
       </c>
-      <c r="F82" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="13">
         <v>43810</v>
       </c>
@@ -6308,11 +6056,8 @@
       <c r="E83" s="15">
         <v>17472</v>
       </c>
-      <c r="F83" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="13">
         <v>43815</v>
       </c>
@@ -6328,11 +6073,8 @@
       <c r="E84" s="15">
         <v>18591</v>
       </c>
-      <c r="F84" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="13">
         <v>43808</v>
       </c>
@@ -6348,11 +6090,8 @@
       <c r="E85" s="15">
         <v>19602.7</v>
       </c>
-      <c r="F85" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="13">
         <v>43801</v>
       </c>
@@ -6368,11 +6107,8 @@
       <c r="E86" s="15">
         <v>20000</v>
       </c>
-      <c r="F86" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="13">
         <v>43816</v>
       </c>
@@ -6388,11 +6124,8 @@
       <c r="E87" s="15">
         <v>20000</v>
       </c>
-      <c r="F87" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="13">
         <v>43818</v>
       </c>
@@ -6408,11 +6141,8 @@
       <c r="E88" s="15">
         <v>20000</v>
       </c>
-      <c r="F88" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="13">
         <v>43817</v>
       </c>
@@ -6428,11 +6158,8 @@
       <c r="E89" s="15">
         <v>20016</v>
       </c>
-      <c r="F89" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="13">
         <v>43817</v>
       </c>
@@ -6448,11 +6175,8 @@
       <c r="E90" s="15">
         <v>20016</v>
       </c>
-      <c r="F90" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="13">
         <v>43818</v>
       </c>
@@ -6468,11 +6192,8 @@
       <c r="E91" s="15">
         <v>20241</v>
       </c>
-      <c r="F91" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="13">
         <v>43815</v>
       </c>
@@ -6488,11 +6209,8 @@
       <c r="E92" s="15">
         <v>22000</v>
       </c>
-      <c r="F92" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="13">
         <v>43808</v>
       </c>
@@ -6508,11 +6226,8 @@
       <c r="E93" s="15">
         <v>26926</v>
       </c>
-      <c r="F93" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="13">
         <v>43809</v>
       </c>
@@ -6528,11 +6243,8 @@
       <c r="E94" s="15">
         <v>28193.05</v>
       </c>
-      <c r="F94" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="13">
         <v>43802</v>
       </c>
@@ -6548,11 +6260,8 @@
       <c r="E95" s="15">
         <v>28856</v>
       </c>
-      <c r="F95" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="13">
         <v>43816</v>
       </c>
@@ -6568,11 +6277,8 @@
       <c r="E96" s="15">
         <v>29000</v>
       </c>
-      <c r="F96" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="13">
         <v>43815</v>
       </c>
@@ -6588,11 +6294,8 @@
       <c r="E97" s="15">
         <v>29854.65</v>
       </c>
-      <c r="F97" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="13">
         <v>43819</v>
       </c>
@@ -6608,11 +6311,8 @@
       <c r="E98" s="15">
         <v>30058</v>
       </c>
-      <c r="F98" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="13">
         <v>43809</v>
       </c>
@@ -6628,11 +6328,8 @@
       <c r="E99" s="15">
         <v>30193.200000000001</v>
       </c>
-      <c r="F99" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="13">
         <v>43802</v>
       </c>
@@ -6646,11 +6343,8 @@
       <c r="E100" s="15">
         <v>30549</v>
       </c>
-      <c r="F100" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="13">
         <v>43801</v>
       </c>
@@ -6664,11 +6358,8 @@
       <c r="E101" s="15">
         <v>30940</v>
       </c>
-      <c r="F101" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="13">
         <v>43801</v>
       </c>
@@ -6684,11 +6375,8 @@
       <c r="E102" s="15">
         <v>31215</v>
       </c>
-      <c r="F102" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="13">
         <v>43812</v>
       </c>
@@ -6704,11 +6392,8 @@
       <c r="E103" s="15">
         <v>32116</v>
       </c>
-      <c r="F103" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="13">
         <v>43815</v>
       </c>
@@ -6724,11 +6409,8 @@
       <c r="E104" s="15">
         <v>32310</v>
       </c>
-      <c r="F104" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="13">
         <v>43816</v>
       </c>
@@ -6744,11 +6426,8 @@
       <c r="E105" s="15">
         <v>32340</v>
       </c>
-      <c r="F105" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="13">
         <v>43801</v>
       </c>
@@ -6764,11 +6443,8 @@
       <c r="E106" s="15">
         <v>33000</v>
       </c>
-      <c r="F106" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="13">
         <v>43816</v>
       </c>
@@ -6784,11 +6460,8 @@
       <c r="E107" s="15">
         <v>34550</v>
       </c>
-      <c r="F107" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="13">
         <v>43810</v>
       </c>
@@ -6804,11 +6477,8 @@
       <c r="E108" s="15">
         <v>35319.65</v>
       </c>
-      <c r="F108" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="13">
         <v>43815</v>
       </c>
@@ -6824,11 +6494,8 @@
       <c r="E109" s="15">
         <v>36180</v>
       </c>
-      <c r="F109" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="13">
         <v>43819</v>
       </c>
@@ -6844,11 +6511,8 @@
       <c r="E110" s="15">
         <v>36682</v>
       </c>
-      <c r="F110" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="13">
         <v>43809</v>
       </c>
@@ -6864,11 +6528,8 @@
       <c r="E111" s="15">
         <v>36820</v>
       </c>
-      <c r="F111" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="13">
         <v>43816</v>
       </c>
@@ -6884,11 +6545,8 @@
       <c r="E112" s="15">
         <v>40000</v>
       </c>
-      <c r="F112" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="13">
         <v>43803</v>
       </c>
@@ -6904,11 +6562,8 @@
       <c r="E113" s="15">
         <v>40216</v>
       </c>
-      <c r="F113" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="13">
         <v>43820</v>
       </c>
@@ -6924,11 +6579,8 @@
       <c r="E114" s="15">
         <v>40726</v>
       </c>
-      <c r="F114" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="13">
         <v>43817</v>
       </c>
@@ -6944,11 +6596,8 @@
       <c r="E115" s="15">
         <v>42000</v>
       </c>
-      <c r="F115" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="13">
         <v>43822</v>
       </c>
@@ -6964,11 +6613,8 @@
       <c r="E116" s="15">
         <v>42124.2</v>
       </c>
-      <c r="F116" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="13">
         <v>43804</v>
       </c>
@@ -6984,11 +6630,8 @@
       <c r="E117" s="15">
         <v>45911</v>
       </c>
-      <c r="F117" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="13">
         <v>43809</v>
       </c>
@@ -7004,11 +6647,8 @@
       <c r="E118" s="15">
         <v>49645.599999999999</v>
       </c>
-      <c r="F118" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="13">
         <v>43813</v>
       </c>
@@ -7024,11 +6664,8 @@
       <c r="E119" s="15">
         <v>56861</v>
       </c>
-      <c r="F119" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="13">
         <v>43801</v>
       </c>
@@ -7044,11 +6681,8 @@
       <c r="E120" s="15">
         <v>57128</v>
       </c>
-      <c r="F120" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="13">
         <v>43813</v>
       </c>
@@ -7064,11 +6698,8 @@
       <c r="E121" s="15">
         <v>57236</v>
       </c>
-      <c r="F121" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="13">
         <v>43801</v>
       </c>
@@ -7084,11 +6715,8 @@
       <c r="E122" s="15">
         <v>59017.7</v>
       </c>
-      <c r="F122" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="13">
         <v>43809</v>
       </c>
@@ -7104,11 +6732,8 @@
       <c r="E123" s="15">
         <v>60000</v>
       </c>
-      <c r="F123" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="13">
         <v>43817</v>
       </c>
@@ -7124,11 +6749,8 @@
       <c r="E124" s="15">
         <v>60142.95</v>
       </c>
-      <c r="F124" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="13">
         <v>43810</v>
       </c>
@@ -7144,11 +6766,8 @@
       <c r="E125" s="15">
         <v>60370</v>
       </c>
-      <c r="F125" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="13">
         <v>43801</v>
       </c>
@@ -7162,11 +6781,8 @@
       <c r="E126" s="15">
         <v>62735</v>
       </c>
-      <c r="F126" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="13">
         <v>43819</v>
       </c>
@@ -7182,11 +6798,8 @@
       <c r="E127" s="15">
         <v>63762</v>
       </c>
-      <c r="F127" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="13">
         <v>43808</v>
       </c>
@@ -7202,11 +6815,8 @@
       <c r="E128" s="15">
         <v>64142</v>
       </c>
-      <c r="F128" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="13">
         <v>43815</v>
       </c>
@@ -7222,11 +6832,8 @@
       <c r="E129" s="15">
         <v>64704</v>
       </c>
-      <c r="F129" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" s="29" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:5" s="29" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="25">
         <v>43812</v>
       </c>
@@ -7242,11 +6849,8 @@
       <c r="E130" s="28">
         <v>65542</v>
       </c>
-      <c r="F130" s="29" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="13">
         <v>43805</v>
       </c>
@@ -7262,11 +6866,8 @@
       <c r="E131" s="15">
         <v>67800</v>
       </c>
-      <c r="F131" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="13">
         <v>43822</v>
       </c>
@@ -7282,11 +6883,8 @@
       <c r="E132" s="15">
         <v>69000</v>
       </c>
-      <c r="F132" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="13">
         <v>43815</v>
       </c>
@@ -7302,11 +6900,8 @@
       <c r="E133" s="15">
         <v>69536.399999999994</v>
       </c>
-      <c r="F133" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="13">
         <v>43808</v>
       </c>
@@ -7322,11 +6917,8 @@
       <c r="E134" s="15">
         <v>70981</v>
       </c>
-      <c r="F134" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="13">
         <v>43809</v>
       </c>
@@ -7342,11 +6934,8 @@
       <c r="E135" s="15">
         <v>75152.600000000006</v>
       </c>
-      <c r="F135" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="13">
         <v>43801</v>
       </c>
@@ -7362,11 +6951,8 @@
       <c r="E136" s="15">
         <v>76000</v>
       </c>
-      <c r="F136" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="13">
         <v>43808</v>
       </c>
@@ -7382,11 +6968,8 @@
       <c r="E137" s="15">
         <v>80209.3</v>
       </c>
-      <c r="F137" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="13">
         <v>43818</v>
       </c>
@@ -7402,11 +6985,8 @@
       <c r="E138" s="15">
         <v>90000</v>
       </c>
-      <c r="F138" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="13">
         <v>43812</v>
       </c>
@@ -7422,11 +7002,8 @@
       <c r="E139" s="15">
         <v>91000</v>
       </c>
-      <c r="F139" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="13">
         <v>43801</v>
       </c>
@@ -7442,11 +7019,8 @@
       <c r="E140" s="15">
         <v>98308.6</v>
       </c>
-      <c r="F140" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="13">
         <v>43804</v>
       </c>
@@ -7462,11 +7036,8 @@
       <c r="E141" s="15">
         <v>98610</v>
       </c>
-      <c r="F141" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="13">
         <v>43804</v>
       </c>
@@ -7482,11 +7053,8 @@
       <c r="E142" s="15">
         <v>100000</v>
       </c>
-      <c r="F142" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="13">
         <v>43805</v>
       </c>
@@ -7502,11 +7070,8 @@
       <c r="E143" s="15">
         <v>100000</v>
       </c>
-      <c r="F143" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="13">
         <v>43816</v>
       </c>
@@ -7522,11 +7087,8 @@
       <c r="E144" s="15">
         <v>113249</v>
       </c>
-      <c r="F144" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="13">
         <v>43815</v>
       </c>
@@ -7542,11 +7104,8 @@
       <c r="E145" s="15">
         <v>113412</v>
       </c>
-      <c r="F145" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="13">
         <v>43804</v>
       </c>
@@ -7562,11 +7121,8 @@
       <c r="E146" s="15">
         <v>121449</v>
       </c>
-      <c r="F146" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="13">
         <v>43801</v>
       </c>
@@ -7582,11 +7138,8 @@
       <c r="E147" s="15">
         <v>121583.65</v>
       </c>
-      <c r="F147" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="13">
         <v>43802</v>
       </c>
@@ -7602,11 +7155,8 @@
       <c r="E148" s="15">
         <v>147420.75</v>
       </c>
-      <c r="F148" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="13">
         <v>43808</v>
       </c>
@@ -7622,11 +7172,8 @@
       <c r="E149" s="15">
         <v>159004</v>
       </c>
-      <c r="F149" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="13">
         <v>43801</v>
       </c>
@@ -7640,11 +7187,8 @@
       <c r="E150" s="15">
         <v>188205</v>
       </c>
-      <c r="F150" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="13">
         <v>43803</v>
       </c>
@@ -7660,11 +7204,8 @@
       <c r="E151" s="15">
         <v>217000</v>
       </c>
-      <c r="F151" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="13">
         <v>43810</v>
       </c>
@@ -7680,11 +7221,8 @@
       <c r="E152" s="15">
         <v>353550</v>
       </c>
-      <c r="F152" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="13">
         <v>43801</v>
       </c>
@@ -7700,11 +7238,8 @@
       <c r="E153" s="15">
         <v>379332.5</v>
       </c>
-      <c r="F153" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="13">
         <v>43803</v>
       </c>
@@ -7720,16 +7255,8 @@
       <c r="E154" s="15">
         <v>3310027.25</v>
       </c>
-      <c r="F154" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F155" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="156" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="13">
         <v>43822</v>
       </c>
@@ -7745,11 +7272,8 @@
       <c r="E156" s="15">
         <v>10000</v>
       </c>
-      <c r="F156" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="157" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="13">
         <v>43822</v>
       </c>
@@ -7765,11 +7289,8 @@
       <c r="E157" s="15">
         <v>860</v>
       </c>
-      <c r="F157" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="13">
         <v>43822</v>
       </c>
@@ -7785,11 +7306,8 @@
       <c r="E158" s="15">
         <v>10400</v>
       </c>
-      <c r="F158" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="159" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="13">
         <v>43822</v>
       </c>
@@ -7805,11 +7323,8 @@
       <c r="E159" s="15">
         <v>21066</v>
       </c>
-      <c r="F159" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="13">
         <v>43822</v>
       </c>
@@ -7825,11 +7340,8 @@
       <c r="E160" s="15">
         <v>860</v>
       </c>
-      <c r="F160" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="161" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="13">
         <v>43822</v>
       </c>
@@ -7845,11 +7357,8 @@
       <c r="E161" s="15">
         <v>860</v>
       </c>
-      <c r="F161" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="162" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="13">
         <v>43822</v>
       </c>
@@ -7865,11 +7374,8 @@
       <c r="E162" s="15">
         <v>860</v>
       </c>
-      <c r="F162" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="163" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="13">
         <v>43822</v>
       </c>
@@ -7885,11 +7391,8 @@
       <c r="E163" s="15">
         <v>860</v>
       </c>
-      <c r="F163" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="164" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="13">
         <v>43822</v>
       </c>
@@ -7905,11 +7408,8 @@
       <c r="E164" s="15">
         <v>860</v>
       </c>
-      <c r="F164" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="165" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="13">
         <v>43822</v>
       </c>
@@ -7925,11 +7425,8 @@
       <c r="E165" s="15">
         <v>860</v>
       </c>
-      <c r="F165" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="166" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="13">
         <v>43822</v>
       </c>
@@ -7945,11 +7442,8 @@
       <c r="E166" s="15">
         <v>860</v>
       </c>
-      <c r="F166" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="167" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="13">
         <v>43822</v>
       </c>
@@ -7965,11 +7459,8 @@
       <c r="E167" s="15">
         <v>860</v>
       </c>
-      <c r="F167" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="168" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="13">
         <v>43822</v>
       </c>
@@ -7985,11 +7476,8 @@
       <c r="E168" s="15">
         <v>860</v>
       </c>
-      <c r="F168" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="169" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="13">
         <v>43822</v>
       </c>
@@ -8005,11 +7493,8 @@
       <c r="E169" s="15">
         <v>860</v>
       </c>
-      <c r="F169" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="170" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="13">
         <v>43822</v>
       </c>
@@ -8025,11 +7510,8 @@
       <c r="E170" s="15">
         <v>860</v>
       </c>
-      <c r="F170" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="171" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="13">
         <v>43822</v>
       </c>
@@ -8045,11 +7527,8 @@
       <c r="E171" s="15">
         <v>860</v>
       </c>
-      <c r="F171" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="172" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="13">
         <v>43822</v>
       </c>
@@ -8065,11 +7544,8 @@
       <c r="E172" s="15">
         <v>860</v>
       </c>
-      <c r="F172" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="173" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="13">
         <v>43822</v>
       </c>
@@ -8085,11 +7561,8 @@
       <c r="E173" s="15">
         <v>109870</v>
       </c>
-      <c r="F173" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="174" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="13">
         <v>43822</v>
       </c>
@@ -8105,11 +7578,8 @@
       <c r="E174" s="15">
         <v>4976</v>
       </c>
-      <c r="F174" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="175" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="13">
         <v>43822</v>
       </c>
@@ -8125,11 +7595,8 @@
       <c r="E175" s="15">
         <v>6100</v>
       </c>
-      <c r="F175" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="176" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="13">
         <v>43822</v>
       </c>
@@ -8145,11 +7612,8 @@
       <c r="E176" s="15">
         <v>6094</v>
       </c>
-      <c r="F176" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="177" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="13">
         <v>43822</v>
       </c>
@@ -8165,11 +7629,8 @@
       <c r="E177" s="15">
         <v>20000</v>
       </c>
-      <c r="F177" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="178" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="13">
         <v>43822</v>
       </c>
@@ -8185,11 +7646,8 @@
       <c r="E178" s="15">
         <v>6100</v>
       </c>
-      <c r="F178" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="179" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="13">
         <v>43823</v>
       </c>
@@ -8205,11 +7663,8 @@
       <c r="E179" s="15">
         <v>15480</v>
       </c>
-      <c r="F179" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="180" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="13">
         <v>43823</v>
       </c>
@@ -8225,11 +7680,8 @@
       <c r="E180" s="15">
         <v>88351</v>
       </c>
-      <c r="F180" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="181" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="13">
         <v>43823</v>
       </c>
@@ -8245,11 +7697,8 @@
       <c r="E181" s="15">
         <v>58170</v>
       </c>
-      <c r="F181" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="182" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="13">
         <v>43823</v>
       </c>
@@ -8265,11 +7714,8 @@
       <c r="E182" s="15">
         <v>2580</v>
       </c>
-      <c r="F182" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="183" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="13">
         <v>43823</v>
       </c>
@@ -8285,11 +7731,8 @@
       <c r="E183" s="15">
         <v>6210</v>
       </c>
-      <c r="F183" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="184" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="13">
         <v>43823</v>
       </c>
@@ -8305,11 +7748,8 @@
       <c r="E184" s="15">
         <v>59017.7</v>
       </c>
-      <c r="F184" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="185" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A185" s="13">
         <v>43823</v>
       </c>
@@ -8325,11 +7765,8 @@
       <c r="E185" s="15">
         <v>5879</v>
       </c>
-      <c r="F185" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="186" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A186" s="13">
         <v>43823</v>
       </c>
@@ -8345,11 +7782,8 @@
       <c r="E186" s="15">
         <v>5907</v>
       </c>
-      <c r="F186" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="187" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A187" s="13">
         <v>43823</v>
       </c>
@@ -8365,11 +7799,8 @@
       <c r="E187" s="15">
         <v>84772.2</v>
       </c>
-      <c r="F187" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="188" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="13">
         <v>43823</v>
       </c>
@@ -8385,11 +7816,8 @@
       <c r="E188" s="15">
         <v>2369.6999999999998</v>
       </c>
-      <c r="F188" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="189" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="13">
         <v>43823</v>
       </c>
@@ -8405,11 +7833,8 @@
       <c r="E189" s="15">
         <v>106000</v>
       </c>
-      <c r="F189" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="190" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A190" s="13">
         <v>43823</v>
       </c>
@@ -8425,11 +7850,8 @@
       <c r="E190" s="15">
         <v>8392</v>
       </c>
-      <c r="F190" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="191" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="13">
         <v>43823</v>
       </c>
@@ -8445,11 +7867,8 @@
       <c r="E191" s="15">
         <v>3833</v>
       </c>
-      <c r="F191" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="192" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="13">
         <v>43823</v>
       </c>
@@ -8465,11 +7884,8 @@
       <c r="E192" s="15">
         <v>1340</v>
       </c>
-      <c r="F192" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="193" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="13">
         <v>43823</v>
       </c>
@@ -8485,11 +7901,8 @@
       <c r="E193" s="15">
         <v>860</v>
       </c>
-      <c r="F193" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="194" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="13">
         <v>43823</v>
       </c>
@@ -8505,11 +7918,8 @@
       <c r="E194" s="15">
         <v>860</v>
       </c>
-      <c r="F194" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="195" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A195" s="13">
         <v>43823</v>
       </c>
@@ -8525,11 +7935,8 @@
       <c r="E195" s="15">
         <v>860</v>
       </c>
-      <c r="F195" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="196" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A196" s="13">
         <v>43823</v>
       </c>
@@ -8545,11 +7952,8 @@
       <c r="E196" s="15">
         <v>860</v>
       </c>
-      <c r="F196" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="197" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A197" s="13">
         <v>43823</v>
       </c>
@@ -8565,11 +7969,8 @@
       <c r="E197" s="15">
         <v>860</v>
       </c>
-      <c r="F197" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="198" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="13">
         <v>43823</v>
       </c>
@@ -8585,11 +7986,8 @@
       <c r="E198" s="15">
         <v>860</v>
       </c>
-      <c r="F198" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="199" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="13">
         <v>43823</v>
       </c>
@@ -8605,11 +8003,8 @@
       <c r="E199" s="15">
         <v>860</v>
       </c>
-      <c r="F199" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="200" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A200" s="13">
         <v>43823</v>
       </c>
@@ -8625,11 +8020,8 @@
       <c r="E200" s="15">
         <v>860</v>
       </c>
-      <c r="F200" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="201" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A201" s="13">
         <v>43823</v>
       </c>
@@ -8645,11 +8037,8 @@
       <c r="E201" s="15">
         <v>860</v>
       </c>
-      <c r="F201" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="202" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A202" s="13">
         <v>43823</v>
       </c>
@@ -8665,11 +8054,8 @@
       <c r="E202" s="15">
         <v>860</v>
       </c>
-      <c r="F202" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="203" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="13">
         <v>43823</v>
       </c>
@@ -8685,11 +8071,8 @@
       <c r="E203" s="15">
         <v>860</v>
       </c>
-      <c r="F203" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="204" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="13">
         <v>43823</v>
       </c>
@@ -8705,11 +8088,8 @@
       <c r="E204" s="15">
         <v>860</v>
       </c>
-      <c r="F204" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="205" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A205" s="13">
         <v>43823</v>
       </c>
@@ -8725,11 +8105,8 @@
       <c r="E205" s="15">
         <v>860</v>
       </c>
-      <c r="F205" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="206" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A206" s="13">
         <v>43823</v>
       </c>
@@ -8745,11 +8122,8 @@
       <c r="E206" s="15">
         <v>860</v>
       </c>
-      <c r="F206" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="207" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A207" s="13">
         <v>43823</v>
       </c>
@@ -8765,11 +8139,8 @@
       <c r="E207" s="15">
         <v>860</v>
       </c>
-      <c r="F207" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="208" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="13">
         <v>43823</v>
       </c>
@@ -8785,11 +8156,8 @@
       <c r="E208" s="15">
         <v>860</v>
       </c>
-      <c r="F208" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="209" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="13">
         <v>43823</v>
       </c>
@@ -8805,11 +8173,8 @@
       <c r="E209" s="15">
         <v>860</v>
       </c>
-      <c r="F209" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="210" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="13">
         <v>43823</v>
       </c>
@@ -8825,11 +8190,8 @@
       <c r="E210" s="15">
         <v>860</v>
       </c>
-      <c r="F210" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="211" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A211" s="13">
         <v>43823</v>
       </c>
@@ -8845,11 +8207,8 @@
       <c r="E211" s="15">
         <v>33386</v>
       </c>
-      <c r="F211" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="212" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="13">
         <v>43823</v>
       </c>
@@ -8865,11 +8224,8 @@
       <c r="E212" s="15">
         <v>63228</v>
       </c>
-      <c r="F212" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="213" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="13">
         <v>43823</v>
       </c>
@@ -8885,11 +8241,8 @@
       <c r="E213" s="15">
         <v>63228</v>
       </c>
-      <c r="F213" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="214" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A214" s="13">
         <v>43823</v>
       </c>
@@ -8905,11 +8258,8 @@
       <c r="E214" s="15">
         <v>150000</v>
       </c>
-      <c r="F214" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="215" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A215" s="13">
         <v>43823</v>
       </c>
@@ -8925,11 +8275,8 @@
       <c r="E215" s="15">
         <v>181365</v>
       </c>
-      <c r="F215" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="216" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A216" s="13">
         <v>43823</v>
       </c>
@@ -8945,11 +8292,8 @@
       <c r="E216" s="15">
         <v>860</v>
       </c>
-      <c r="F216" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="217" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A217" s="13">
         <v>43823</v>
       </c>
@@ -8965,11 +8309,8 @@
       <c r="E217" s="15">
         <v>63228</v>
       </c>
-      <c r="F217" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="218" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="13">
         <v>43823</v>
       </c>
@@ -8985,11 +8326,8 @@
       <c r="E218" s="15">
         <v>78696</v>
       </c>
-      <c r="F218" s="16">
-        <v>90182</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="219" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A219" s="13">
         <v>43823</v>
       </c>
@@ -9005,11 +8343,8 @@
       <c r="E219" s="15">
         <v>860</v>
       </c>
-      <c r="F219" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="220" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A220" s="13">
         <v>43823</v>
       </c>
@@ -9025,11 +8360,8 @@
       <c r="E220" s="15">
         <v>860</v>
       </c>
-      <c r="F220" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="221" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="13">
         <v>43823</v>
       </c>
@@ -9045,11 +8377,8 @@
       <c r="E221" s="15">
         <v>860</v>
       </c>
-      <c r="F221" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="222" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="13">
         <v>43823</v>
       </c>
@@ -9065,11 +8394,8 @@
       <c r="E222" s="15">
         <v>860</v>
       </c>
-      <c r="F222" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="223" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A223" s="13">
         <v>43823</v>
       </c>
@@ -9085,11 +8411,8 @@
       <c r="E223" s="15">
         <v>20124</v>
       </c>
-      <c r="F223" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="224" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A224" s="13">
         <v>43823</v>
       </c>
@@ -9105,11 +8428,8 @@
       <c r="E224" s="15">
         <v>2580</v>
       </c>
-      <c r="F224" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="225" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A225" s="13">
         <v>43823</v>
       </c>
@@ -9125,11 +8445,8 @@
       <c r="E225" s="15">
         <v>21600</v>
       </c>
-      <c r="F225" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="226" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A226" s="13">
         <v>43823</v>
       </c>
@@ -9145,11 +8462,8 @@
       <c r="E226" s="15">
         <v>7200</v>
       </c>
-      <c r="F226" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="227" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A227" s="13">
         <v>43823</v>
       </c>
@@ -9165,11 +8479,8 @@
       <c r="E227" s="15">
         <v>85996</v>
       </c>
-      <c r="F227" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="228" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A228" s="13">
         <v>43826</v>
       </c>
@@ -9185,11 +8496,8 @@
       <c r="E228" s="15">
         <v>54587.7</v>
       </c>
-      <c r="F228" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="229" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A229" s="13">
         <v>43826</v>
       </c>
@@ -9205,11 +8513,8 @@
       <c r="E229" s="15">
         <v>4763.6499999999996</v>
       </c>
-      <c r="F229" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="230" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A230" s="13">
         <v>43826</v>
       </c>
@@ -9225,11 +8530,8 @@
       <c r="E230" s="15">
         <v>19602.7</v>
       </c>
-      <c r="F230" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="231" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A231" s="13">
         <v>43826</v>
       </c>
@@ -9245,11 +8547,8 @@
       <c r="E231" s="15">
         <v>20313.75</v>
       </c>
-      <c r="F231" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="232" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A232" s="13">
         <v>43826</v>
       </c>
@@ -9265,11 +8564,8 @@
       <c r="E232" s="15">
         <v>75152.600000000006</v>
       </c>
-      <c r="F232" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="233" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A233" s="13">
         <v>43826</v>
       </c>
@@ -9285,11 +8581,8 @@
       <c r="E233" s="15">
         <v>30193.200000000001</v>
       </c>
-      <c r="F233" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="234" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A234" s="13">
         <v>43826</v>
       </c>
@@ -9305,11 +8598,8 @@
       <c r="E234" s="15">
         <v>2580</v>
       </c>
-      <c r="F234" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="235" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="13">
         <v>43826</v>
       </c>
@@ -9325,11 +8615,8 @@
       <c r="E235" s="15">
         <v>3440</v>
       </c>
-      <c r="F235" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="236" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A236" s="13">
         <v>43826</v>
       </c>
@@ -9345,16 +8632,8 @@
       <c r="E236" s="15">
         <v>89777</v>
       </c>
-      <c r="F236" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F237" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="238" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A238" s="13">
         <v>43826</v>
       </c>
@@ -9370,11 +8649,8 @@
       <c r="E238" s="15">
         <v>-78696</v>
       </c>
-      <c r="F238" s="16">
-        <v>90182</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="239" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A239" s="13">
         <v>43830</v>
       </c>
@@ -9390,11 +8666,8 @@
       <c r="E239" s="15">
         <v>-8490</v>
       </c>
-      <c r="F239" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="240" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A240" s="13">
         <v>43830</v>
       </c>
@@ -9410,11 +8683,8 @@
       <c r="E240" s="15">
         <v>-1698</v>
       </c>
-      <c r="F240" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="241" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A241" s="13">
         <v>43829</v>
       </c>
@@ -9430,11 +8700,8 @@
       <c r="E241" s="15">
         <v>860</v>
       </c>
-      <c r="F241" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="242" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A242" s="13">
         <v>43829</v>
       </c>
@@ -9450,11 +8717,8 @@
       <c r="E242" s="15">
         <v>860</v>
       </c>
-      <c r="F242" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="243" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A243" s="13">
         <v>43829</v>
       </c>
@@ -9470,11 +8734,8 @@
       <c r="E243" s="15">
         <v>860</v>
       </c>
-      <c r="F243" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="244" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A244" s="13">
         <v>43829</v>
       </c>
@@ -9490,11 +8751,8 @@
       <c r="E244" s="15">
         <v>860</v>
       </c>
-      <c r="F244" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="245" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="13">
         <v>43829</v>
       </c>
@@ -9510,11 +8768,8 @@
       <c r="E245" s="15">
         <v>860</v>
       </c>
-      <c r="F245" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="246" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="13">
         <v>43829</v>
       </c>
@@ -9530,11 +8785,8 @@
       <c r="E246" s="15">
         <v>860</v>
       </c>
-      <c r="F246" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="247" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="13">
         <v>43829</v>
       </c>
@@ -9550,11 +8802,8 @@
       <c r="E247" s="15">
         <v>860</v>
       </c>
-      <c r="F247" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="248" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="13">
         <v>43829</v>
       </c>
@@ -9570,11 +8819,8 @@
       <c r="E248" s="15">
         <v>860</v>
       </c>
-      <c r="F248" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="249" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="13">
         <v>43829</v>
       </c>
@@ -9590,11 +8836,8 @@
       <c r="E249" s="15">
         <v>860</v>
       </c>
-      <c r="F249" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="250" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="13">
         <v>43829</v>
       </c>
@@ -9610,11 +8853,8 @@
       <c r="E250" s="15">
         <v>860</v>
       </c>
-      <c r="F250" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="251" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="13">
         <v>43829</v>
       </c>
@@ -9630,11 +8870,8 @@
       <c r="E251" s="15">
         <v>860</v>
       </c>
-      <c r="F251" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="252" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="13">
         <v>43829</v>
       </c>
@@ -9650,11 +8887,8 @@
       <c r="E252" s="15">
         <v>860</v>
       </c>
-      <c r="F252" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="253" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="13">
         <v>43829</v>
       </c>
@@ -9670,11 +8904,8 @@
       <c r="E253" s="15">
         <v>860</v>
       </c>
-      <c r="F253" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="254" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="13">
         <v>43829</v>
       </c>
@@ -9690,11 +8921,8 @@
       <c r="E254" s="15">
         <v>860</v>
       </c>
-      <c r="F254" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="255" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="13">
         <v>43830</v>
       </c>
@@ -9710,11 +8938,8 @@
       <c r="E255" s="15">
         <v>860</v>
       </c>
-      <c r="F255" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="256" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="13">
         <v>43830</v>
       </c>
@@ -9730,11 +8955,8 @@
       <c r="E256" s="15">
         <v>1720</v>
       </c>
-      <c r="F256" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="257" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="13">
         <v>43830</v>
       </c>
@@ -9750,11 +8972,8 @@
       <c r="E257" s="15">
         <v>1720</v>
       </c>
-      <c r="F257" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="258" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="13">
         <v>43830</v>
       </c>
@@ -9770,11 +8989,8 @@
       <c r="E258" s="15">
         <v>1940</v>
       </c>
-      <c r="F258" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="259" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="13">
         <v>43830</v>
       </c>
@@ -9790,11 +9006,8 @@
       <c r="E259" s="15">
         <v>1981</v>
       </c>
-      <c r="F259" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="260" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A260" s="13">
         <v>43829</v>
       </c>
@@ -9810,11 +9023,8 @@
       <c r="E260" s="15">
         <v>2547.1999999999998</v>
       </c>
-      <c r="F260" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="261" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A261" s="13">
         <v>43829</v>
       </c>
@@ -9830,11 +9040,8 @@
       <c r="E261" s="15">
         <v>2547.1999999999998</v>
       </c>
-      <c r="F261" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="262" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A262" s="13">
         <v>43829</v>
       </c>
@@ -9850,11 +9057,8 @@
       <c r="E262" s="15">
         <v>3155.4</v>
       </c>
-      <c r="F262" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="263" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="263" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A263" s="13">
         <v>43830</v>
       </c>
@@ -9870,11 +9074,8 @@
       <c r="E263" s="15">
         <v>4300</v>
       </c>
-      <c r="F263" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="264" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A264" s="13">
         <v>43829</v>
       </c>
@@ -9890,11 +9091,8 @@
       <c r="E264" s="15">
         <v>4980</v>
       </c>
-      <c r="F264" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="265" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A265" s="13">
         <v>43829</v>
       </c>
@@ -9910,11 +9108,8 @@
       <c r="E265" s="15">
         <v>6000</v>
       </c>
-      <c r="F265" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="266" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="266" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="13">
         <v>43830</v>
       </c>
@@ -9930,11 +9125,8 @@
       <c r="E266" s="15">
         <v>6019</v>
       </c>
-      <c r="F266" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="267" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A267" s="13">
         <v>43830</v>
       </c>
@@ -9950,11 +9142,8 @@
       <c r="E267" s="15">
         <v>6039</v>
       </c>
-      <c r="F267" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="268" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="13">
         <v>43832</v>
       </c>
@@ -9970,11 +9159,8 @@
       <c r="E268" s="15">
         <v>6725</v>
       </c>
-      <c r="F268" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="269" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="13">
         <v>43829</v>
       </c>
@@ -9990,11 +9176,8 @@
       <c r="E269" s="15">
         <v>7500</v>
       </c>
-      <c r="F269" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="270" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="13">
         <v>43829</v>
       </c>
@@ -10010,11 +9193,8 @@
       <c r="E270" s="15">
         <v>11095</v>
       </c>
-      <c r="F270" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="271" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A271" s="13">
         <v>43830</v>
       </c>
@@ -10030,11 +9210,8 @@
       <c r="E271" s="15">
         <v>11101</v>
       </c>
-      <c r="F271" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="272" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A272" s="13">
         <v>43829</v>
       </c>
@@ -10050,11 +9227,8 @@
       <c r="E272" s="15">
         <v>17637</v>
       </c>
-      <c r="F272" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="273" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A273" s="13">
         <v>43829</v>
       </c>
@@ -10070,11 +9244,8 @@
       <c r="E273" s="15">
         <v>20000</v>
       </c>
-      <c r="F273" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="274" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A274" s="13">
         <v>43829</v>
       </c>
@@ -10090,11 +9261,8 @@
       <c r="E274" s="15">
         <v>20076</v>
       </c>
-      <c r="F274" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="275" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="275" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A275" s="13">
         <v>43826</v>
       </c>
@@ -10110,11 +9278,8 @@
       <c r="E275" s="15">
         <v>22120</v>
       </c>
-      <c r="F275" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="276" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="276" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A276" s="13">
         <v>43827</v>
       </c>
@@ -10130,11 +9295,8 @@
       <c r="E276" s="15">
         <v>26618</v>
       </c>
-      <c r="F276" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="277" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="277" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A277" s="13">
         <v>43829</v>
       </c>
@@ -10150,11 +9312,8 @@
       <c r="E277" s="15">
         <v>27502</v>
       </c>
-      <c r="F277" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="278" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="278" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A278" s="13">
         <v>43830</v>
       </c>
@@ -10170,11 +9329,8 @@
       <c r="E278" s="15">
         <v>28856</v>
       </c>
-      <c r="F278" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="279" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="279" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A279" s="13">
         <v>43830</v>
       </c>
@@ -10190,11 +9346,8 @@
       <c r="E279" s="15">
         <v>32610</v>
       </c>
-      <c r="F279" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="280" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="280" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="13">
         <v>43830</v>
       </c>
@@ -10210,11 +9363,8 @@
       <c r="E280" s="15">
         <v>39137.839999999997</v>
       </c>
-      <c r="F280" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="281" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="281" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A281" s="13">
         <v>43830</v>
       </c>
@@ -10230,11 +9380,8 @@
       <c r="E281" s="15">
         <v>42100</v>
       </c>
-      <c r="F281" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="282" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A282" s="13">
         <v>43830</v>
       </c>
@@ -10250,11 +9397,8 @@
       <c r="E282" s="15">
         <v>49645.599999999999</v>
       </c>
-      <c r="F282" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="283" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A283" s="13">
         <v>43830</v>
       </c>
@@ -10270,11 +9414,8 @@
       <c r="E283" s="15">
         <v>61421</v>
       </c>
-      <c r="F283" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="284" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A284" s="13">
         <v>43829</v>
       </c>
@@ -10290,11 +9431,8 @@
       <c r="E284" s="15">
         <v>63402</v>
       </c>
-      <c r="F284" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="285" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A285" s="13">
         <v>43829</v>
       </c>
@@ -10310,11 +9448,8 @@
       <c r="E285" s="15">
         <v>64748</v>
       </c>
-      <c r="F285" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="286" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="286" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A286" s="13">
         <v>43826</v>
       </c>
@@ -10330,11 +9465,8 @@
       <c r="E286" s="15">
         <v>78696</v>
       </c>
-      <c r="F286" s="16" t="s">
-        <v>1376</v>
-      </c>
-    </row>
-    <row r="287" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="287" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A287" s="13">
         <v>43829</v>
       </c>
@@ -10350,11 +9482,8 @@
       <c r="E287" s="15">
         <v>87727.85</v>
       </c>
-      <c r="F287" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="288" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="288" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A288" s="13">
         <v>43832</v>
       </c>
@@ -10370,11 +9499,8 @@
       <c r="E288" s="15">
         <v>100000</v>
       </c>
-      <c r="F288" s="16" t="s">
-        <v>1375</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="289" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A289" s="13">
         <v>43830</v>
       </c>
@@ -10390,11 +9516,8 @@
       <c r="E289" s="15">
         <v>121583.65</v>
       </c>
-      <c r="F289" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="290" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A290" s="13">
         <v>43830</v>
       </c>
@@ -10410,11 +9533,8 @@
       <c r="E290" s="15">
         <v>155179.79999999999</v>
       </c>
-      <c r="F290" s="16" t="s">
-        <v>1377</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="291" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A291" s="13">
         <v>43829</v>
       </c>
@@ -10429,9 +9549,6 @@
       </c>
       <c r="E291" s="15">
         <v>389324.45</v>
-      </c>
-      <c r="F291" s="16" t="s">
-        <v>1377</v>
       </c>
     </row>
   </sheetData>
@@ -10446,8 +9563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E469"/>
   <sheetViews>
-    <sheetView topLeftCell="A412" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>